<commit_message>
Add sample codes using Google test framework with global variables.
</commit_message>
<xml_diff>
--- a/doc/sample/test_sample_input/google_test_sample_data.xlsx
+++ b/doc/sample/test_sample_input/google_test_sample_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="テスト一覧" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="107">
   <si>
     <t>○対象関数情報</t>
     <rPh sb="1" eb="7">
@@ -570,6 +570,21 @@
   </si>
   <si>
     <t>subFuncA_002_subInput1[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>sample_function_004</t>
+  </si>
+  <si>
+    <t>sample_src.cpp</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>sample_src.cpp</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>sample_function_004</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1116,7 +1131,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="V49" sqref="V49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1192,14 +1209,22 @@
         <v>65</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -4176,7 +4201,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4244,7 +4271,7 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">

</xml_diff>

<commit_message>
Update sample code and test data for utest using Googletest framework.
</commit_message>
<xml_diff>
--- a/doc/sample/test_sample_input/google_test_sample_data.xlsx
+++ b/doc/sample/test_sample_input/google_test_sample_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882"/>
   </bookViews>
   <sheets>
     <sheet name="テスト一覧" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="123">
   <si>
     <t>○対象関数情報</t>
     <rPh sb="1" eb="7">
@@ -585,6 +585,76 @@
   </si>
   <si>
     <t>sample_function_004</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>input2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&amp;input2[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>_input2[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>_input2[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>_input2[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>非NULL</t>
+    <rPh sb="0" eb="1">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>input2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&amp;_input2[0]</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>非NULL</t>
+    <rPh sb="0" eb="1">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>A</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -702,7 +772,17 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <border>
+        <top/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1131,9 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="V49" sqref="V49"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3270,7 +3348,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AC27"/>
+  <dimension ref="B2:AC28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
@@ -3289,9 +3367,9 @@
     <col min="12" max="12" width="2.375" style="5" customWidth="1"/>
     <col min="13" max="13" width="9.625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="45" width="3" style="5" customWidth="1"/>
     <col min="46" max="16384" width="2.125" style="5"/>
   </cols>
@@ -3641,9 +3719,11 @@
         <v>3</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P15" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
       <c r="Q15" s="6">
         <v>0</v>
       </c>
@@ -3686,7 +3766,7 @@
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -3699,26 +3779,50 @@
         <v>3</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>0</v>
-      </c>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B17" s="8"/>
@@ -3735,32 +3839,24 @@
         <v>3</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Q17" s="6">
-        <v>1</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-      <c r="U17" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
-      <c r="X17" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
-      <c r="AA17" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
     </row>
@@ -3779,33 +3875,33 @@
         <v>3</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q18" s="6">
-        <v>2</v>
-      </c>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="U18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V18" s="3"/>
       <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="X18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="AA18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.15">
@@ -3823,76 +3919,86 @@
         <v>3</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>42</v>
       </c>
       <c r="Q19" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3" t="s">
+      <c r="S19" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3" t="s">
+      <c r="V19" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="Y19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="AB19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC19" s="3"/>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="M20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P20" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Q20" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
+      <c r="T20" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
+      <c r="W20" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
+      <c r="Z20" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
+      <c r="AC20" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="8"/>
       <c r="M21" s="3" t="s">
         <v>36</v>
@@ -3905,29 +4011,17 @@
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="6">
-        <v>1</v>
-      </c>
-      <c r="R21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="S21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
       <c r="U21" s="3"/>
-      <c r="V21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="W21" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
-      <c r="Z21" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
@@ -3951,36 +4045,36 @@
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="6">
-        <v>2</v>
-      </c>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y22" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3" t="s">
+      <c r="T22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AB22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC22" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -3997,20 +4091,32 @@
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="U23" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
+      <c r="X23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y23" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
+      <c r="AA23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC23" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B24" s="8"/>
@@ -4024,37 +4130,31 @@
         <v>36</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-      <c r="U24" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
-      <c r="AC24" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="AC24" s="3"/>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -4071,30 +4171,26 @@
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="6">
-        <v>10</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3" t="s">
+      <c r="U25" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="V25" s="3"/>
       <c r="W25" s="3"/>
-      <c r="X25" s="3" t="s">
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
-      <c r="AB25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.15">
       <c r="B26" s="8"/>
@@ -4115,28 +4211,39 @@
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="6">
-        <v>20</v>
-      </c>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R26" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3" t="s">
+      <c r="V26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="X26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3" t="s">
+      <c r="Z26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="AB26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AC26" s="3"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.15">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
       <c r="M27" s="3" t="s">
         <v>36</v>
       </c>
@@ -4148,48 +4255,81 @@
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
-      <c r="T27" s="3" t="s">
+      <c r="S27" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
+      <c r="W27" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-      <c r="AA27" s="3"/>
+      <c r="AA27" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
     </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.15">
+      <c r="M28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="6">
+        <v>30</v>
+      </c>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C4:D7 M21:P23 M11:P15 M17:O19">
+  <conditionalFormatting sqref="C4:D7 M22:P24 M11:P16 M18:P20">
     <cfRule type="expression" dxfId="6" priority="4">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:P27">
+  <conditionalFormatting sqref="M25:P28">
     <cfRule type="expression" dxfId="5" priority="2">
-      <formula>M24=M23</formula>
+      <formula>M25=M24</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20:P20">
+  <conditionalFormatting sqref="M21:P21">
     <cfRule type="expression" dxfId="4" priority="6">
-      <formula>M20=#REF!</formula>
+      <formula>M21=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M16:O16">
+  <conditionalFormatting sqref="M17:O17">
     <cfRule type="expression" dxfId="3" priority="8">
-      <formula>M16=#REF!</formula>
+      <formula>M17=#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P16:P19">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>P16=P15</formula>
+  <conditionalFormatting sqref="P17">
+    <cfRule type="expression" dxfId="0" priority="15">
+      <formula>P17=P15</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4199,11 +4339,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X28"/>
+  <dimension ref="B2:Y29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4218,21 +4356,21 @@
     <col min="10" max="10" width="14.375" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.125" style="5"/>
     <col min="12" max="12" width="2.375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="9.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.875" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.25" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="24" width="2.5" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="2.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
@@ -4258,7 +4396,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
@@ -4278,7 +4416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
@@ -4298,7 +4436,7 @@
       </c>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
@@ -4320,7 +4458,7 @@
       </c>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
@@ -4338,7 +4476,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
@@ -4360,7 +4498,7 @@
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C9" s="6" t="s">
         <v>46</v>
       </c>
@@ -4378,7 +4516,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.15">
       <c r="C10" s="6" t="s">
         <v>46</v>
       </c>
@@ -4396,12 +4534,12 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.15">
       <c r="L12" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.15">
       <c r="M13" s="11" t="s">
         <v>37</v>
       </c>
@@ -4423,13 +4561,26 @@
       <c r="S13" s="4">
         <v>2</v>
       </c>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="T13" s="4">
+        <v>3</v>
+      </c>
+      <c r="U13" s="4">
+        <v>4</v>
+      </c>
+      <c r="V13" s="4">
+        <v>5</v>
+      </c>
+      <c r="W13" s="4">
+        <v>6</v>
+      </c>
+      <c r="X13" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.15">
       <c r="M14" s="3" t="s">
         <v>35</v>
       </c>
@@ -4445,17 +4596,20 @@
       <c r="Q14" s="6">
         <v>0</v>
       </c>
-      <c r="R14" s="3"/>
+      <c r="R14" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="S14" s="3" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y14" s="3"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -4480,13 +4634,18 @@
       </c>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
+      <c r="T15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y15" s="3"/>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -4513,11 +4672,16 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
+      <c r="V16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="X16" s="3"/>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y16" s="3"/>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -4546,9 +4710,14 @@
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="X17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -4563,7 +4732,7 @@
         <v>3</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>40</v>
@@ -4571,15 +4740,20 @@
       <c r="Q18" s="6">
         <v>0</v>
       </c>
-      <c r="R18" s="3"/>
+      <c r="R18" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
+      <c r="T18" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y18" s="3"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -4594,7 +4768,7 @@
         <v>3</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>40</v>
@@ -4603,14 +4777,19 @@
         <v>1</v>
       </c>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="S19" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
+      <c r="U19" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y19" s="3"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
       <c r="D20" s="8"/>
@@ -4625,7 +4804,7 @@
         <v>3</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="P20" s="3" t="s">
         <v>42</v>
@@ -4634,16 +4813,19 @@
         <v>2</v>
       </c>
       <c r="R20" s="3"/>
-      <c r="S20" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
+      <c r="V20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="X20" s="3"/>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y20" s="3"/>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="8"/>
@@ -4658,7 +4840,7 @@
         <v>3</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>42</v>
@@ -4672,44 +4854,68 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="X21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="M22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="6">
-        <v>0</v>
-      </c>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.15">
+        <v>107</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="8"/>
       <c r="M23" s="3" t="s">
         <v>36</v>
@@ -4722,17 +4928,22 @@
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="6">
-        <v>1</v>
-      </c>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y23" s="3"/>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -4751,21 +4962,24 @@
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R24" s="3"/>
-      <c r="S24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y24" s="3"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -4782,17 +4996,22 @@
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
+      <c r="V25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="W25" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="X25" s="3"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="Y25" s="3"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="8"/>
@@ -4800,17 +5019,42 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="M26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="6">
+        <v>3</v>
+      </c>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -4819,16 +5063,25 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.15">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="C4:D10">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="C4:D10 M24:P26 M14:P22">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:P25">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>M14=M13</formula>
+  <conditionalFormatting sqref="M23:P23">
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>M23=M21</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update samples. Add "sample_function_005" to google_test_sample_data.xlsx. This is to show code the application will generate if the data type of argument in test target function is void with pointer.
</commit_message>
<xml_diff>
--- a/doc/sample/test_sample_input/google_test_sample_data.xlsx
+++ b/doc/sample/test_sample_input/google_test_sample_data.xlsx
@@ -12,13 +12,14 @@
     <sheet name="sample_function_002" sheetId="3" r:id="rId3"/>
     <sheet name="sample_function_003" sheetId="6" r:id="rId4"/>
     <sheet name="sample_function_004" sheetId="7" r:id="rId5"/>
+    <sheet name="sample_function_005" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="139">
   <si>
     <t>○対象関数情報</t>
     <rPh sb="1" eb="7">
@@ -687,6 +688,18 @@
   </si>
   <si>
     <t>*</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>sample_function_005</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>VOID</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>sample_function_005</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1174,9 +1187,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1267,6 +1282,20 @@
       </c>
       <c r="F7" s="2" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2957,7 +2986,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D6 M10:P23">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4095,7 +4124,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D6 M10:P27">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6047,7 +6076,905 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C4:D6 M10:P40">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>C4=C3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AG23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="2.125" style="5"/>
+    <col min="3" max="3" width="10.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.125" style="5"/>
+    <col min="12" max="12" width="2.375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="9.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="33" width="3" style="5" customWidth="1"/>
+    <col min="34" max="16384" width="2.125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="L8" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="M9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="4">
+        <v>1</v>
+      </c>
+      <c r="S9" s="4">
+        <v>2</v>
+      </c>
+      <c r="T9" s="4">
+        <v>3</v>
+      </c>
+      <c r="U9" s="4">
+        <v>4</v>
+      </c>
+      <c r="V9" s="4">
+        <v>5</v>
+      </c>
+      <c r="W9" s="4">
+        <v>6</v>
+      </c>
+      <c r="X9" s="4">
+        <v>7</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>9</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>10</v>
+      </c>
+      <c r="AB9" s="4">
+        <v>11</v>
+      </c>
+      <c r="AC9" s="4">
+        <v>12</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>13</v>
+      </c>
+      <c r="AE9" s="4">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>15</v>
+      </c>
+      <c r="AG9" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="M10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+    </row>
+    <row r="11" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="M11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+    </row>
+    <row r="12" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="8"/>
+      <c r="M12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>2</v>
+      </c>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="M13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>3</v>
+      </c>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="M14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="M15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" s="6">
+        <v>0</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="M16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>1</v>
+      </c>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+    </row>
+    <row r="17" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="M17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>2</v>
+      </c>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG17" s="3"/>
+    </row>
+    <row r="18" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="M18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>3</v>
+      </c>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="M19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="8"/>
+      <c r="M20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="6">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="M21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="6">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG21" s="3"/>
+    </row>
+    <row r="22" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="M22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="6">
+        <v>2</v>
+      </c>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+    </row>
+    <row r="23" spans="2:33" x14ac:dyDescent="0.15">
+      <c r="M23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="6">
+        <v>3</v>
+      </c>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <conditionalFormatting sqref="C4:D6 M10:P23">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>C4=C3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>